<commit_message>
AUTH API - Updated the authentication methods
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>API - End points</t>
   </si>
@@ -46,14 +46,6 @@
   </si>
   <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
- "name":"Zeeshan",
- "email":"zeeshanahmedd0010@gmail.com",
- "password":"zee1234"
-}
-</t>
   </si>
   <si>
     <t>Text</t>
@@ -84,6 +76,19 @@
   </si>
   <si>
     <t>/authenticationService/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+{
+ "displayName":"Zeeshan",
+ "email":"zeeshanahmedd0010@gmail.com",
+ "password":"zee1234",
+ "phoneNumber":"+923053206339",
+ "profileURL":"",
+ "onlineStatus":"Active",
+ "address":"no where"
+}
+</t>
   </si>
 </sst>
 </file>
@@ -469,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +486,7 @@
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="49.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="69" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
@@ -538,12 +543,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -552,13 +557,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
@@ -566,27 +571,32 @@
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H7" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created-EndPoint-RestPasswordViaEmail and Updated the created account method so that it may send verfication email
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>API - End points</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>accountsService/createAccountWithEmail</t>
-  </si>
-  <si>
-    <t>this will create account in firebase authentication and connected mysql</t>
   </si>
   <si>
     <t>Authentication</t>
@@ -90,12 +87,32 @@
 }
 </t>
   </si>
+  <si>
+    <t>accountsService/restMyPasswordWithEmailLink</t>
+  </si>
+  <si>
+    <t>to reset password via email</t>
+  </si>
+  <si>
+    <t>{
+ "email":"zeeshanahmedd0010@gmail.com"
+}</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>this send an email for password varaification</t>
+  </si>
+  <si>
+    <t>this will create account in firebase and will send the email varification link and will not allow until u verifiy your account</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +142,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -152,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -171,6 +194,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +499,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,13 +581,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
@@ -578,25 +602,48 @@
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the response formates
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -48,9 +48,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>accountsService/createAccountWithEmail</t>
   </si>
   <si>
@@ -106,6 +103,15 @@
   </si>
   <si>
     <t>this will create account in firebase and will send the email varification link and will not allow until u verifiy your account</t>
+  </si>
+  <si>
+    <t>{
+    "responseMessage": {
+        "code": "auth/email-already-exists",
+        "message": "The email address is already in use by another account."
+    },
+    "responseCode": 4
+}</t>
   </si>
 </sst>
 </file>
@@ -188,13 +194,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,43 +515,43 @@
     <col min="4" max="4" width="29.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="49.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="78.7109375" customWidth="1"/>
     <col min="8" max="8" width="69" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -572,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -581,13 +587,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
@@ -602,48 +608,48 @@
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created endpoint : addToContactList
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G32" sqref="G28:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the Xcel file
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>API - End points</t>
   </si>
@@ -181,6 +181,157 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>profileService/loadProfileWithUid</t>
+  </si>
+  <si>
+    <t>to load profile with uid</t>
+  </si>
+  <si>
+    <t>{
+ "uid":"Apj5bwYRadRxNcjR3Wwm2urBSj22"
+{
+ "uid":"Apj5bwYRadRxNcjR3Wwm2urBSj22"
+}</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>chatService/addInContactListrout</t>
+  </si>
+  <si>
+    <t>to add any user in contact list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "userUid":"4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+ "contactUserUid":"Apj5bwYRadRxNcjR3Wwm2urBSj22",
+ "contactUserName":"Ahmed",
+ "contactUserProfile":"https://firebasestorage.googleapis.com/v0/b/discussion-manager.appspot.com/o/1620937610218-WhatsApp%20Image%202021-04-07%20at%203.00.32%20AM.jpeg?alt=media&amp;token=49ee247d-98bd-4719-8220-3ddd561b3ada"
+}
+</t>
+  </si>
+  <si>
+    <t>{
+    "responseMessage": "Record Added",
+    "responseCode": 1
+}</t>
+  </si>
+  <si>
+    <t>chatService/loadAllContacts</t>
+  </si>
+  <si>
+    <t>to loadd list of contacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "uid":"0TFdiLUfj8Vq0Qtoz14jAhNuGu03"
+}
+</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "contactUserUid": "4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+        "contactUserName": "Shan",
+        "contactUserProfile": "https://firebasestorage.googleapis.com/v0/b/discussion-manager.appspot.com/o/1620937610218-WhatsApp%20Image%202021-04-07%20at%203.00.32%20AM.jpeg?alt=media&amp;token=49ee247d-98bd-4719-8220-3ddd561b3ada"
+    },
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "contactUserUid": "Apj5bwYRadRxNcjR3Wwm2urBSj22",
+        "contactUserName": "Ahmed",
+        "contactUserProfile": "https://firebasestorage.googleapis.com/v0/b/discussion-manager.appspot.com/o/1620937610218-WhatsApp%20Image%202021-04-07%20at%203.00.32%20AM.jpeg?alt=media&amp;token=49ee247d-98bd-4719-8220-3ddd561b3ada"
+    },
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "contactUserUid": "LFu2IhjTGZb2YjflHY9kVrVzXFh2",
+        "contactUserName": "Zee",
+        "contactUserProfile": "https://firebasestorage.googleapis.com/v0/b/discussion-manager.appspot.com/o/1620937610218-WhatsApp%20Image%202021-04-07%20at%203.00.32%20AM.jpeg?alt=media&amp;token=49ee247d-98bd-4719-8220-3ddd561b3ada"
+    }
+]</t>
+  </si>
+  <si>
+    <t>chatService/sendMessage</t>
+  </si>
+  <si>
+    <t>to send message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "userUid":"0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+ "recieverUid":"4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+ "messageType":"Text",
+ "messageContent":"who ree you",
+ "messageStatus":"New",
+ "messageSendTime":"23:51:19.60 14/05/2021" 
+}
+</t>
+  </si>
+  <si>
+    <t>{
+    "responseMessage": "Message Sent",
+    "responseCode": 1
+}</t>
+  </si>
+  <si>
+    <t>chatService/loadChat</t>
+  </si>
+  <si>
+    <t>to load chat with some limit</t>
+  </si>
+  <si>
+    <t>{
+ "userUid":"0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+ "recieverUid":"4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+ "numberOfMessages":"4",
+ "messageOffset":"0"
+}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "userUid": "4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+        "recieverUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "messageType": "Text",
+        "messageContent": "i am zee",
+        "messageStatus": "Seen",
+        "messageSendTime": " 23:49:51.",
+        "serialNumber": 6
+    },
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "recieverUid": "4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+        "messageType": "Text",
+        "messageContent": "who ree you",
+        "messageStatus": "Seen",
+        "messageSendTime": "23:51:19.6",
+        "serialNumber": 5
+    },
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "recieverUid": "4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+        "messageType": "Text",
+        "messageContent": "who ree you",
+        "messageStatus": "Seen",
+        "messageSendTime": "23:51:19.6",
+        "serialNumber": 4
+    },
+    {
+        "userUid": "0TFdiLUfj8Vq0Qtoz14jAhNuGu03",
+        "recieverUid": "4KksC4PFIBe8JKDSDgwu0Q1R3Jv2",
+        "messageType": "Text",
+        "messageContent": "who ree you",
+        "messageStatus": "New",
+        "messageSendTime": "23:51:19.6",
+        "serialNumber": 3
+    }
+]</t>
   </si>
 </sst>
 </file>
@@ -571,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G32" sqref="G28:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +734,7 @@
     <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="67" customWidth="1"/>
     <col min="7" max="7" width="78.7109375" customWidth="1"/>
     <col min="8" max="8" width="69" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -780,8 +931,105 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Created the new request list and connnected it with database
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
done with chating module
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -187,13 +187,6 @@
   </si>
   <si>
     <t>to load profile with uid</t>
-  </si>
-  <si>
-    <t>{
- "uid":"Apj5bwYRadRxNcjR3Wwm2urBSj22"
-{
- "uid":"Apj5bwYRadRxNcjR3Wwm2urBSj22"
-}</t>
   </si>
   <si>
     <t>Same as above</t>
@@ -332,6 +325,11 @@
         "serialNumber": 3
     }
 ]</t>
+  </si>
+  <si>
+    <t>{
+ "uid":"Apj5bwYRadRxNcjR3Wwm2urBSj22"
+}</t>
   </si>
 </sst>
 </file>
@@ -724,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -945,90 +943,90 @@
         <v>9</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
         <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
         <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved issue with end point creation
</commit_message>
<xml_diff>
--- a/API-End-Points/api-end-points.xlsx
+++ b/API-End-Points/api-end-points.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>API - End points</t>
   </si>
@@ -332,6 +332,31 @@
         "serialNumber": 3
     }
 ]</t>
+  </si>
+  <si>
+    <t>Posts</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/postsServices/addPost</t>
+  </si>
+  <si>
+    <t>to upload the posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "userUid":"5U9wbAfe66RrFRibw07u9qBkDQJ2",
+ "postTitle":"Post 1",
+ "postImage":"https://firebasestorage.googleapis.com/v0/b/discussion-manager.appspot.com/o/annie-spratt-QckxruozjRg-unsplash.jpg?alt=media&amp;token=922ba71c-45dd-4f46-85ba-6030eb80cea9",
+ "sentTimeDate":"7:50",
+ "postDesc":"New post desc"
+}
+</t>
+  </si>
+  <si>
+    <t>{
+    "responseMessage": "Uploaded the post",
+    "responseCode": 2
+}</t>
   </si>
 </sst>
 </file>
@@ -722,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,6 +1054,26 @@
       </c>
       <c r="G17" s="7" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>